<commit_message>
New version of Allegro games
</commit_message>
<xml_diff>
--- a/georgia_tech_courses.xlsx
+++ b/georgia_tech_courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ldsmith\college_work\GeorgiaTechProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E512A062-93CA-45C3-A7EB-4F18A16AFFD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E431BDA6-7A3C-4B23-9944-F30EA094BFB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{29BD3D7B-D4D1-48BD-8059-018E6C25E8AD}"/>
+    <workbookView xWindow="11550" yWindow="405" windowWidth="28800" windowHeight="19770" xr2:uid="{29BD3D7B-D4D1-48BD-8059-018E6C25E8AD}"/>
   </bookViews>
   <sheets>
     <sheet name="GeorgiaTech" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="155">
   <si>
     <t>CMPE 1700</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>Bill Beavers</t>
+  </si>
+  <si>
+    <t>Russ Shackelford?</t>
   </si>
 </sst>
 </file>
@@ -873,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B2A32D-8C9E-4559-9988-7EC03201F5F8}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,6 +953,9 @@
       <c r="B8" t="s">
         <v>11</v>
       </c>
+      <c r="C8" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1341,7 +1347,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1349,7 +1355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3197C83-728A-4751-A331-0EA9B7976D0C}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>

</xml_diff>